<commit_message>
Add Reset Password Endpoint
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/src/main/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/src/main/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="136">
   <si>
     <t>de_DE</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>new_course_registration_requested</t>
+  </si>
+  <si>
+    <t>user_password_request_reset_success</t>
   </si>
 </sst>
 </file>
@@ -829,7 +832,7 @@
   <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1375,6 +1378,9 @@
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>135</v>
+      </c>
       <c r="B51" s="2"/>
       <c r="C51" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update Mail notification templates
</commit_message>
<xml_diff>
--- a/platform/microservices/trust-certification-system-gateway-api/src/main/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/trust-certification-system-gateway-api/src/main/resources/i18n/translation_default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="217">
   <si>
     <t>de_DE</t>
   </si>
@@ -589,6 +589,87 @@
   </si>
   <si>
     <t>{0}, Your request to issue a certificate {1} has been rejected!</t>
+  </si>
+  <si>
+    <t>mail_ca_enabled_body</t>
+  </si>
+  <si>
+    <t>{0}, Your account as CA has been successfully enabled, now you can register new courses and issuer new certificates</t>
+  </si>
+  <si>
+    <t>{0}, Tu cuenta como CA ha sido habilitada exitosamente, ahora puedes dar de alta nuevos cursos y emitir nuevos certificados</t>
+  </si>
+  <si>
+    <t>mail_ca_disabled_body</t>
+  </si>
+  <si>
+    <t>{0}, Tu cuenta como CA ha sido deshabilitada, no podrás registrar nuevos cursos ni emitir nuevos certificados hasta que sea activada de nuevo.</t>
+  </si>
+  <si>
+    <t>{0}, Your CA account has been disabled, you will not be able to register new courses or issue new certificates until it is activated again.</t>
+  </si>
+  <si>
+    <t>mail_certificate_disabled_body</t>
+  </si>
+  <si>
+    <t>{0}, Tú certificado {1} ha sido deshabilitado, este no podrá ser renovado ni utilizado hasta que sea habilitado de nuevo.</t>
+  </si>
+  <si>
+    <t>{0}, Your certificate {1} has been disabled, it cannot be renewed or used until it is enabled again.</t>
+  </si>
+  <si>
+    <t>mail_certificate_enabled_body</t>
+  </si>
+  <si>
+    <t>{0}, Tú certificado {1} ha sido habilitado, podrás renovar y utilizar tu certificado con normalidad.</t>
+  </si>
+  <si>
+    <t>{0}, Your certificate {1} has been enabled, you can renew and use your certificate normally.</t>
+  </si>
+  <si>
+    <t>mail_certificate_renewed_body</t>
+  </si>
+  <si>
+    <t>mail_certificate_request_accepted_body</t>
+  </si>
+  <si>
+    <t>{0}, Tú certificado {1} ha sido renovado, podrás seguir utilizándolo con normalidad.</t>
+  </si>
+  <si>
+    <t>{0}, Your certificate {1} has been renewed, you can continue to use it normally.</t>
+  </si>
+  <si>
+    <t>{0}, Tú solicitud de emisión del certificado {1} ha sido aceptada, en breve tú certificado será generado y almacenado en TCS.</t>
+  </si>
+  <si>
+    <t>{0}, Your request to issue the certificate {1} has been accepted, shortly your certificate will be generated and stored in TCS.</t>
+  </si>
+  <si>
+    <t>{0}, Tú solicitud de emisión del certificado {1} ha sido rechazada.</t>
+  </si>
+  <si>
+    <t>{0}, Your request to issue the certificate {1} has been rejected.</t>
+  </si>
+  <si>
+    <t>mail_certificate_request_rejected_body</t>
+  </si>
+  <si>
+    <t>mail_certificate_changed_to_visible_body</t>
+  </si>
+  <si>
+    <t>mail_certificate_changed_to_invisible_body</t>
+  </si>
+  <si>
+    <t>{0}, The visibility of your certificate {1} has been updated, your certificate is now visible.</t>
+  </si>
+  <si>
+    <t>{0}, La visibilidad de tú certificado {1} ha sido actualizada, tú certificado ahora es visible.</t>
+  </si>
+  <si>
+    <t>{0}, La visibilidad de tú certificado {1} ha sido actualizada, tú certificado ahora no es visible.</t>
+  </si>
+  <si>
+    <t>{0}, The visibility of your certificate {1} has been updated, your certificate is now not visible.</t>
   </si>
 </sst>
 </file>
@@ -996,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1728,34 +1809,103 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-      <c r="C66" s="5"/>
+      <c r="A66" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="5"/>
+      <c r="A67" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
-      <c r="C68" s="4"/>
+      <c r="A68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
-      <c r="C69" s="4"/>
+      <c r="A69" t="s">
+        <v>199</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
-      <c r="C70" s="4"/>
+      <c r="A70" t="s">
+        <v>202</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
-      <c r="C71" s="4"/>
+      <c r="A71" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="4"/>
+      <c r="A72" t="s">
+        <v>210</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C74" s="4"/>
+      <c r="A74" t="s">
+        <v>212</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>216</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>